<commit_message>
Fix Excel file, adding zeroes
</commit_message>
<xml_diff>
--- a/server/data.xlsx
+++ b/server/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/PTDL2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44E23EA-7F07-2D45-8025-1C155FF76F6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A40B85-63A6-2A40-AF16-7140B6E80F91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15320" yWindow="760" windowWidth="10000" windowHeight="17400" xr2:uid="{97A7DAB1-8DC6-8A44-8B1A-1933BBBAF9F6}"/>
+    <workbookView xWindow="100" yWindow="740" windowWidth="25220" windowHeight="17400" activeTab="1" xr2:uid="{97A7DAB1-8DC6-8A44-8B1A-1933BBBAF9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Dư nợ tín dụng" sheetId="1" r:id="rId1"/>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60B2805-03D0-EE4A-A3A1-A01D561D1AC1}">
   <dimension ref="A1:S132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -893,7 +893,7 @@
         <v>4.05</v>
       </c>
       <c r="F8">
-        <v>87154</v>
+        <v>871540</v>
       </c>
       <c r="G8">
         <v>2.34</v>
@@ -911,7 +911,7 @@
         <v>-6.4</v>
       </c>
       <c r="L8">
-        <v>57811</v>
+        <v>578110</v>
       </c>
       <c r="M8">
         <v>-6.39</v>
@@ -1011,7 +1011,7 @@
         <v>4.83</v>
       </c>
       <c r="F10">
-        <v>88251</v>
+        <v>882510</v>
       </c>
       <c r="G10">
         <v>3.79</v>
@@ -1141,7 +1141,7 @@
         <v>1.83</v>
       </c>
       <c r="J12">
-        <v>72203</v>
+        <v>722030</v>
       </c>
       <c r="K12">
         <v>-1.92</v>
@@ -1306,7 +1306,7 @@
         <v>2.67</v>
       </c>
       <c r="F15">
-        <v>93219</v>
+        <v>932190</v>
       </c>
       <c r="G15">
         <v>3.01</v>
@@ -1365,7 +1365,7 @@
         <v>2.67</v>
       </c>
       <c r="F16">
-        <v>9268</v>
+        <v>926800</v>
       </c>
       <c r="G16">
         <v>2.42</v>
@@ -1377,7 +1377,7 @@
         <v>3.45</v>
       </c>
       <c r="J16">
-        <v>72599</v>
+        <v>725990</v>
       </c>
       <c r="K16">
         <v>-1.39</v>
@@ -1424,7 +1424,7 @@
         <v>3.34</v>
       </c>
       <c r="F17">
-        <v>93039</v>
+        <v>930390</v>
       </c>
       <c r="G17">
         <v>2.81</v>
@@ -1489,7 +1489,7 @@
         <v>4.75</v>
       </c>
       <c r="H18">
-        <v>30557</v>
+        <v>305570</v>
       </c>
       <c r="I18">
         <v>6.18</v>
@@ -1501,7 +1501,7 @@
         <v>0.79</v>
       </c>
       <c r="L18">
-        <v>60876</v>
+        <v>608760</v>
       </c>
       <c r="M18">
         <v>0.81</v>
@@ -1743,7 +1743,7 @@
         <v>5.96</v>
       </c>
       <c r="N22">
-        <v>12657</v>
+        <v>126570</v>
       </c>
       <c r="O22">
         <v>-4.34</v>
@@ -1796,7 +1796,7 @@
         <v>8.51</v>
       </c>
       <c r="L23">
-        <v>67204</v>
+        <v>672040</v>
       </c>
       <c r="M23">
         <v>11.29</v>
@@ -1808,7 +1808,7 @@
         <v>-4.17</v>
       </c>
       <c r="P23">
-        <v>99978</v>
+        <v>999780</v>
       </c>
       <c r="Q23">
         <v>15.7</v>
@@ -1843,7 +1843,7 @@
         <v>-0.67</v>
       </c>
       <c r="H24">
-        <v>3527</v>
+        <v>352700</v>
       </c>
       <c r="I24">
         <v>2.4700000000000002</v>
@@ -1961,7 +1961,7 @@
         <v>1.19</v>
       </c>
       <c r="H26">
-        <v>35062</v>
+        <v>350620</v>
       </c>
       <c r="I26">
         <v>1.86</v>
@@ -2026,7 +2026,7 @@
         <v>1.06</v>
       </c>
       <c r="J27">
-        <v>79474</v>
+        <v>794740</v>
       </c>
       <c r="K27">
         <v>-0.51</v>
@@ -2150,7 +2150,7 @@
         <v>1.18</v>
       </c>
       <c r="L29">
-        <v>68446</v>
+        <v>684460</v>
       </c>
       <c r="M29">
         <v>1.85</v>
@@ -2215,7 +2215,7 @@
         <v>0.95</v>
       </c>
       <c r="N30">
-        <v>12287</v>
+        <v>122870</v>
       </c>
       <c r="O30">
         <v>-3.09</v>
@@ -2268,7 +2268,7 @@
         <v>2.04</v>
       </c>
       <c r="L31">
-        <v>69238</v>
+        <v>692380</v>
       </c>
       <c r="M31">
         <v>3.03</v>
@@ -2333,7 +2333,7 @@
         <v>4.26</v>
       </c>
       <c r="N32">
-        <v>12418</v>
+        <v>124180</v>
       </c>
       <c r="O32">
         <v>-2.06</v>
@@ -2433,7 +2433,7 @@
         <v>6.5</v>
       </c>
       <c r="H34">
-        <v>37011</v>
+        <v>370110</v>
       </c>
       <c r="I34">
         <v>7.52</v>
@@ -2551,7 +2551,7 @@
         <v>0.08</v>
       </c>
       <c r="H36">
-        <v>38306</v>
+        <v>383060</v>
       </c>
       <c r="I36">
         <v>0.7</v>
@@ -2651,7 +2651,7 @@
         <v>42064</v>
       </c>
       <c r="B38">
-        <v>40328</v>
+        <v>403280</v>
       </c>
       <c r="C38">
         <v>3.09</v>
@@ -2728,7 +2728,7 @@
         <v>2.92</v>
       </c>
       <c r="H39">
-        <v>39881</v>
+        <v>398810</v>
       </c>
       <c r="I39">
         <v>4.84</v>
@@ -2793,7 +2793,7 @@
         <v>6.83</v>
       </c>
       <c r="J40">
-        <v>91522</v>
+        <v>915220</v>
       </c>
       <c r="K40">
         <v>4.1399999999999997</v>
@@ -2976,7 +2976,7 @@
         <v>5.54</v>
       </c>
       <c r="L43">
-        <v>77328</v>
+        <v>773280</v>
       </c>
       <c r="M43">
         <v>4.1100000000000003</v>
@@ -3123,7 +3123,7 @@
         <v>42309</v>
       </c>
       <c r="B46">
-        <v>45907</v>
+        <v>459070</v>
       </c>
       <c r="C46">
         <v>17.36</v>
@@ -8215,8 +8215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{083031B0-28AD-ED4A-9976-C49167164E36}">
   <dimension ref="A1:O131"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8303,7 +8303,7 @@
         <v>1449453</v>
       </c>
       <c r="G3">
-        <v>1178</v>
+        <v>11.78</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">

</xml_diff>